<commit_message>
RM-110 Adds authorization check on org_unit for Contract, using new CustomUser.is_authorized_for_org_unit() method
</commit_message>
<xml_diff>
--- a/rm/test/resources/test_total_data_error_empty_rows.xlsx
+++ b/rm/test/resources/test_total_data_error_empty_rows.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t xml:space="preserve">Database nr.</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t xml:space="preserve">ROW ERROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44336</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROW IGNORED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team zonder users</t>
   </si>
 </sst>
 </file>
@@ -172,7 +181,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="[$€-2]\ #,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -200,6 +209,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -251,7 +266,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="1" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -276,6 +291,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -285,6 +304,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF6A8759"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -296,7 +375,7 @@
   <dimension ref="A1:AG1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -306,7 +385,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="6" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="7" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="14.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="12.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="11.5"/>
@@ -592,7 +672,79 @@
         <v>40969.4583333333</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="4" t="n">
+        <v>44256.4583333333</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="5" t="n">
+        <v>2656</v>
+      </c>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="4" t="n">
+        <v>41334.4583333333</v>
+      </c>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG5" s="4" t="n">
+        <v>40969.4583333333</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>